<commit_message>
minor corrections, added annex to index
</commit_message>
<xml_diff>
--- a/annex/draft_workplan/draft_workplan.xlsx
+++ b/annex/draft_workplan/draft_workplan.xlsx
@@ -2,9 +2,9 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26519"/>
-  <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="240" windowWidth="37300" windowHeight="25860" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="19020" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="draft_workplan.csv" sheetId="1" r:id="rId1"/>
@@ -1262,9 +1262,6 @@
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
-  <cols>
-    <col min="2" max="2" width="49.1640625" customWidth="1"/>
-  </cols>
   <sheetData>
     <row r="1" spans="1:20">
       <c r="A1" t="s">
@@ -1336,10 +1333,10 @@
         <v>20</v>
       </c>
       <c r="C2" s="1">
-        <v>42459.333333333336</v>
+        <v>40997.333333333336</v>
       </c>
       <c r="D2" s="1">
-        <v>42517.708333333336</v>
+        <v>41055.708333333336</v>
       </c>
       <c r="E2" t="s">
         <v>21</v>
@@ -1359,10 +1356,10 @@
         <v>23</v>
       </c>
       <c r="C3" s="1">
-        <v>42459.333333333336</v>
+        <v>40997.333333333336</v>
       </c>
       <c r="D3" s="1">
-        <v>42459.708333333336</v>
+        <v>40997.708333333336</v>
       </c>
       <c r="E3" t="s">
         <v>24</v>
@@ -1385,10 +1382,10 @@
         <v>25</v>
       </c>
       <c r="C4" s="1">
-        <v>42459.333333333336</v>
+        <v>40997.333333333336</v>
       </c>
       <c r="D4" s="1">
-        <v>42459.708333333336</v>
+        <v>40997.708333333336</v>
       </c>
       <c r="E4" t="s">
         <v>24</v>
@@ -1411,10 +1408,10 @@
         <v>26</v>
       </c>
       <c r="C5" s="1">
-        <v>42459.333333333336</v>
+        <v>40997.333333333336</v>
       </c>
       <c r="D5" s="1">
-        <v>42459.708333333336</v>
+        <v>40997.708333333336</v>
       </c>
       <c r="E5" t="s">
         <v>24</v>
@@ -1437,10 +1434,10 @@
         <v>27</v>
       </c>
       <c r="C6" s="1">
-        <v>42517.333333333336</v>
+        <v>41055.333333333336</v>
       </c>
       <c r="D6" s="1">
-        <v>42517.708333333336</v>
+        <v>41055.708333333336</v>
       </c>
       <c r="E6" t="s">
         <v>24</v>
@@ -1452,7 +1449,7 @@
         <v>0</v>
       </c>
       <c r="N6" s="1">
-        <v>42517.333333333336</v>
+        <v>41055.333333333336</v>
       </c>
       <c r="R6">
         <v>0</v>
@@ -1466,10 +1463,10 @@
         <v>28</v>
       </c>
       <c r="C7" s="1">
-        <v>42459.333333333336</v>
+        <v>40997.333333333336</v>
       </c>
       <c r="D7" s="1">
-        <v>42459.708333333336</v>
+        <v>40997.708333333336</v>
       </c>
       <c r="E7" t="s">
         <v>24</v>
@@ -1492,10 +1489,10 @@
         <v>29</v>
       </c>
       <c r="C8" s="1">
-        <v>42459.333333333336</v>
+        <v>40997.333333333336</v>
       </c>
       <c r="D8" s="1">
-        <v>42459.708333333336</v>
+        <v>40997.708333333336</v>
       </c>
       <c r="E8" t="s">
         <v>24</v>
@@ -1518,10 +1515,10 @@
         <v>30</v>
       </c>
       <c r="C9" s="1">
-        <v>42459.333333333336</v>
+        <v>40997.333333333336</v>
       </c>
       <c r="D9" s="1">
-        <v>42517.708333333336</v>
+        <v>41055.708333333336</v>
       </c>
       <c r="E9" t="s">
         <v>21</v>
@@ -1541,10 +1538,10 @@
         <v>32</v>
       </c>
       <c r="C10" s="1">
-        <v>42459.333333333336</v>
+        <v>40997.333333333336</v>
       </c>
       <c r="D10" s="1">
-        <v>42459.708333333336</v>
+        <v>40997.708333333336</v>
       </c>
       <c r="E10" t="s">
         <v>24</v>
@@ -1567,10 +1564,10 @@
         <v>33</v>
       </c>
       <c r="C11" s="1">
-        <v>42517.333333333336</v>
+        <v>41055.333333333336</v>
       </c>
       <c r="D11" s="1">
-        <v>42517.708333333336</v>
+        <v>41055.708333333336</v>
       </c>
       <c r="E11" t="s">
         <v>24</v>
@@ -1582,7 +1579,7 @@
         <v>0</v>
       </c>
       <c r="N11" s="1">
-        <v>42517.333333333336</v>
+        <v>41055.333333333336</v>
       </c>
       <c r="R11">
         <v>0</v>
@@ -1596,10 +1593,10 @@
         <v>34</v>
       </c>
       <c r="C12" s="1">
-        <v>42459.333333333336</v>
+        <v>40997.333333333336</v>
       </c>
       <c r="D12" s="1">
-        <v>42459.708333333336</v>
+        <v>40997.708333333336</v>
       </c>
       <c r="E12" t="s">
         <v>24</v>
@@ -1622,10 +1619,10 @@
         <v>35</v>
       </c>
       <c r="C13" s="1">
-        <v>42459.333333333336</v>
+        <v>40997.333333333336</v>
       </c>
       <c r="D13" s="1">
-        <v>42459.708333333336</v>
+        <v>40997.708333333336</v>
       </c>
       <c r="E13" t="s">
         <v>24</v>
@@ -1648,10 +1645,10 @@
         <v>36</v>
       </c>
       <c r="C14" s="1">
-        <v>42459.333333333336</v>
+        <v>40997.333333333336</v>
       </c>
       <c r="D14" s="1">
-        <v>42459.708333333336</v>
+        <v>40997.708333333336</v>
       </c>
       <c r="E14" t="s">
         <v>24</v>
@@ -1674,10 +1671,10 @@
         <v>37</v>
       </c>
       <c r="C15" s="1">
-        <v>42461.333333333336</v>
+        <v>40999.333333333336</v>
       </c>
       <c r="D15" s="1">
-        <v>42517.708333333336</v>
+        <v>41055.708333333336</v>
       </c>
       <c r="E15" t="s">
         <v>38</v>
@@ -1689,7 +1686,7 @@
         <v>0</v>
       </c>
       <c r="N15" s="1">
-        <v>42461.333333333336</v>
+        <v>40999.333333333336</v>
       </c>
     </row>
     <row r="16" spans="1:20">
@@ -1700,10 +1697,10 @@
         <v>40</v>
       </c>
       <c r="C16" s="1">
-        <v>42461.333333333336</v>
+        <v>40999.333333333336</v>
       </c>
       <c r="D16" s="1">
-        <v>42461.708333333336</v>
+        <v>40999.708333333336</v>
       </c>
       <c r="E16" t="s">
         <v>24</v>
@@ -1726,10 +1723,10 @@
         <v>41</v>
       </c>
       <c r="C17" s="1">
-        <v>42517.333333333336</v>
+        <v>41055.333333333336</v>
       </c>
       <c r="D17" s="1">
-        <v>42517.708333333336</v>
+        <v>41055.708333333336</v>
       </c>
       <c r="E17" t="s">
         <v>24</v>
@@ -1741,7 +1738,7 @@
         <v>0</v>
       </c>
       <c r="N17" s="1">
-        <v>42517.333333333336</v>
+        <v>41055.333333333336</v>
       </c>
     </row>
     <row r="18" spans="1:18">
@@ -1752,10 +1749,10 @@
         <v>43</v>
       </c>
       <c r="C18" s="1">
-        <v>42517.333333333336</v>
+        <v>41055.333333333336</v>
       </c>
       <c r="D18" s="1">
-        <v>42517.708333333336</v>
+        <v>41055.708333333336</v>
       </c>
       <c r="E18" t="s">
         <v>24</v>
@@ -1767,7 +1764,7 @@
         <v>0</v>
       </c>
       <c r="N18" s="1">
-        <v>42517.333333333336</v>
+        <v>41055.333333333336</v>
       </c>
       <c r="R18">
         <v>0</v>
@@ -1781,10 +1778,10 @@
         <v>45</v>
       </c>
       <c r="C19" s="1">
-        <v>42517.333333333336</v>
+        <v>41055.333333333336</v>
       </c>
       <c r="D19" s="1">
-        <v>42517.708333333336</v>
+        <v>41055.708333333336</v>
       </c>
       <c r="E19" t="s">
         <v>24</v>
@@ -1796,7 +1793,7 @@
         <v>0</v>
       </c>
       <c r="N19" s="1">
-        <v>42517.333333333336</v>
+        <v>41055.333333333336</v>
       </c>
       <c r="R19">
         <v>0</v>
@@ -1810,10 +1807,10 @@
         <v>47</v>
       </c>
       <c r="C20" s="1">
-        <v>42517.333333333336</v>
+        <v>41055.333333333336</v>
       </c>
       <c r="D20" s="1">
-        <v>42517.708333333336</v>
+        <v>41055.708333333336</v>
       </c>
       <c r="E20" t="s">
         <v>24</v>
@@ -1825,7 +1822,7 @@
         <v>0</v>
       </c>
       <c r="N20" s="1">
-        <v>42517.333333333336</v>
+        <v>41055.333333333336</v>
       </c>
       <c r="R20">
         <v>0</v>
@@ -1839,10 +1836,10 @@
         <v>49</v>
       </c>
       <c r="C21" s="1">
-        <v>42517.333333333336</v>
+        <v>41055.333333333336</v>
       </c>
       <c r="D21" s="1">
-        <v>42517.708333333336</v>
+        <v>41055.708333333336</v>
       </c>
       <c r="E21" t="s">
         <v>24</v>
@@ -1854,7 +1851,7 @@
         <v>0</v>
       </c>
       <c r="N21" s="1">
-        <v>42517.333333333336</v>
+        <v>41055.333333333336</v>
       </c>
       <c r="R21">
         <v>0</v>
@@ -1868,10 +1865,10 @@
         <v>51</v>
       </c>
       <c r="C22" s="1">
-        <v>42517.333333333336</v>
+        <v>41055.333333333336</v>
       </c>
       <c r="D22" s="1">
-        <v>42517.708333333336</v>
+        <v>41055.708333333336</v>
       </c>
       <c r="E22" t="s">
         <v>24</v>
@@ -1883,7 +1880,7 @@
         <v>0</v>
       </c>
       <c r="N22" s="1">
-        <v>42517.333333333336</v>
+        <v>41055.333333333336</v>
       </c>
       <c r="R22">
         <v>0</v>
@@ -1897,10 +1894,10 @@
         <v>52</v>
       </c>
       <c r="C23" s="1">
-        <v>42461.333333333336</v>
+        <v>40999.333333333336</v>
       </c>
       <c r="D23" s="1">
-        <v>42461.708333333336</v>
+        <v>40999.708333333336</v>
       </c>
       <c r="E23" t="s">
         <v>24</v>
@@ -1923,10 +1920,10 @@
         <v>53</v>
       </c>
       <c r="C24" s="1">
-        <v>42461.333333333336</v>
+        <v>40999.333333333336</v>
       </c>
       <c r="D24" s="1">
-        <v>42461.708333333336</v>
+        <v>40999.708333333336</v>
       </c>
       <c r="E24" t="s">
         <v>24</v>
@@ -1949,10 +1946,10 @@
         <v>54</v>
       </c>
       <c r="C25" s="1">
-        <v>42517.333333333336</v>
+        <v>41055.333333333336</v>
       </c>
       <c r="D25" s="1">
-        <v>42517.708333333336</v>
+        <v>41055.708333333336</v>
       </c>
       <c r="E25" t="s">
         <v>24</v>
@@ -1964,7 +1961,7 @@
         <v>0</v>
       </c>
       <c r="N25" s="1">
-        <v>42517.333333333336</v>
+        <v>41055.333333333336</v>
       </c>
       <c r="R25">
         <v>0</v>
@@ -1978,10 +1975,10 @@
         <v>55</v>
       </c>
       <c r="C26" s="1">
-        <v>42461.333333333336</v>
+        <v>40999.333333333336</v>
       </c>
       <c r="D26" s="1">
-        <v>42461.708333333336</v>
+        <v>40999.708333333336</v>
       </c>
       <c r="E26" t="s">
         <v>24</v>
@@ -2004,10 +2001,10 @@
         <v>56</v>
       </c>
       <c r="C27" s="1">
-        <v>42459.333333333336</v>
+        <v>40997.333333333336</v>
       </c>
       <c r="D27" s="1">
-        <v>42517.708333333336</v>
+        <v>41055.708333333336</v>
       </c>
       <c r="E27" t="s">
         <v>21</v>
@@ -2027,10 +2024,10 @@
         <v>58</v>
       </c>
       <c r="C28" s="1">
-        <v>42459.333333333336</v>
+        <v>40997.333333333336</v>
       </c>
       <c r="D28" s="1">
-        <v>42459.708333333336</v>
+        <v>40997.708333333336</v>
       </c>
       <c r="E28" t="s">
         <v>24</v>
@@ -2050,10 +2047,10 @@
         <v>60</v>
       </c>
       <c r="C29" s="1">
-        <v>42459.333333333336</v>
+        <v>40997.333333333336</v>
       </c>
       <c r="D29" s="1">
-        <v>42459.708333333336</v>
+        <v>40997.708333333336</v>
       </c>
       <c r="E29" t="s">
         <v>24</v>
@@ -2076,10 +2073,10 @@
         <v>61</v>
       </c>
       <c r="C30" s="1">
-        <v>42459.333333333336</v>
+        <v>40997.333333333336</v>
       </c>
       <c r="D30" s="1">
-        <v>42459.708333333336</v>
+        <v>40997.708333333336</v>
       </c>
       <c r="E30" t="s">
         <v>24</v>
@@ -2099,10 +2096,10 @@
         <v>64</v>
       </c>
       <c r="C31" s="1">
-        <v>42459.333333333336</v>
+        <v>40997.333333333336</v>
       </c>
       <c r="D31" s="1">
-        <v>42459.708333333336</v>
+        <v>40997.708333333336</v>
       </c>
       <c r="E31" t="s">
         <v>24</v>
@@ -2125,10 +2122,10 @@
         <v>66</v>
       </c>
       <c r="C32" s="1">
-        <v>42459.333333333336</v>
+        <v>40997.333333333336</v>
       </c>
       <c r="D32" s="1">
-        <v>42459.708333333336</v>
+        <v>40997.708333333336</v>
       </c>
       <c r="E32" t="s">
         <v>24</v>
@@ -2151,10 +2148,10 @@
         <v>68</v>
       </c>
       <c r="C33" s="1">
-        <v>42459.333333333336</v>
+        <v>40997.333333333336</v>
       </c>
       <c r="D33" s="1">
-        <v>42459.708333333336</v>
+        <v>40997.708333333336</v>
       </c>
       <c r="E33" t="s">
         <v>24</v>
@@ -2177,10 +2174,10 @@
         <v>70</v>
       </c>
       <c r="C34" s="1">
-        <v>42459.333333333336</v>
+        <v>40997.333333333336</v>
       </c>
       <c r="D34" s="1">
-        <v>42459.708333333336</v>
+        <v>40997.708333333336</v>
       </c>
       <c r="E34" t="s">
         <v>24</v>
@@ -2203,10 +2200,10 @@
         <v>72</v>
       </c>
       <c r="C35" s="1">
-        <v>42459.333333333336</v>
+        <v>40997.333333333336</v>
       </c>
       <c r="D35" s="1">
-        <v>42459.708333333336</v>
+        <v>40997.708333333336</v>
       </c>
       <c r="E35" t="s">
         <v>24</v>
@@ -2229,10 +2226,10 @@
         <v>74</v>
       </c>
       <c r="C36" s="1">
-        <v>42459.333333333336</v>
+        <v>40997.333333333336</v>
       </c>
       <c r="D36" s="1">
-        <v>42459.708333333336</v>
+        <v>40997.708333333336</v>
       </c>
       <c r="E36" t="s">
         <v>24</v>
@@ -2255,10 +2252,10 @@
         <v>76</v>
       </c>
       <c r="C37" s="1">
-        <v>42459.333333333336</v>
+        <v>40997.333333333336</v>
       </c>
       <c r="D37" s="1">
-        <v>42459.708333333336</v>
+        <v>40997.708333333336</v>
       </c>
       <c r="E37" t="s">
         <v>24</v>
@@ -2281,10 +2278,10 @@
         <v>77</v>
       </c>
       <c r="C38" s="1">
-        <v>42459.333333333336</v>
+        <v>40997.333333333336</v>
       </c>
       <c r="D38" s="1">
-        <v>42517.708333333336</v>
+        <v>41055.708333333336</v>
       </c>
       <c r="E38" t="s">
         <v>21</v>
@@ -2304,10 +2301,10 @@
         <v>80</v>
       </c>
       <c r="C39" s="1">
-        <v>42459.333333333336</v>
+        <v>40997.333333333336</v>
       </c>
       <c r="D39" s="1">
-        <v>42459.708333333336</v>
+        <v>40997.708333333336</v>
       </c>
       <c r="E39" t="s">
         <v>24</v>
@@ -2327,10 +2324,10 @@
         <v>82</v>
       </c>
       <c r="C40" s="1">
-        <v>42459.333333333336</v>
+        <v>40997.333333333336</v>
       </c>
       <c r="D40" s="1">
-        <v>42459.708333333336</v>
+        <v>40997.708333333336</v>
       </c>
       <c r="E40" t="s">
         <v>24</v>
@@ -2353,10 +2350,10 @@
         <v>84</v>
       </c>
       <c r="C41" s="1">
-        <v>42459.333333333336</v>
+        <v>40997.333333333336</v>
       </c>
       <c r="D41" s="1">
-        <v>42459.708333333336</v>
+        <v>40997.708333333336</v>
       </c>
       <c r="E41" t="s">
         <v>24</v>
@@ -2379,10 +2376,10 @@
         <v>86</v>
       </c>
       <c r="C42" s="1">
-        <v>42459.333333333336</v>
+        <v>40997.333333333336</v>
       </c>
       <c r="D42" s="1">
-        <v>42459.708333333336</v>
+        <v>40997.708333333336</v>
       </c>
       <c r="E42" t="s">
         <v>24</v>
@@ -2405,10 +2402,10 @@
         <v>88</v>
       </c>
       <c r="C43" s="1">
-        <v>42459.333333333336</v>
+        <v>40997.333333333336</v>
       </c>
       <c r="D43" s="1">
-        <v>42459.708333333336</v>
+        <v>40997.708333333336</v>
       </c>
       <c r="E43" t="s">
         <v>24</v>
@@ -2431,10 +2428,10 @@
         <v>90</v>
       </c>
       <c r="C44" s="1">
-        <v>42459.333333333336</v>
+        <v>40997.333333333336</v>
       </c>
       <c r="D44" s="1">
-        <v>42459.708333333336</v>
+        <v>40997.708333333336</v>
       </c>
       <c r="E44" t="s">
         <v>24</v>
@@ -2457,10 +2454,10 @@
         <v>92</v>
       </c>
       <c r="C45" s="1">
-        <v>42459.333333333336</v>
+        <v>40997.333333333336</v>
       </c>
       <c r="D45" s="1">
-        <v>42459.708333333336</v>
+        <v>40997.708333333336</v>
       </c>
       <c r="E45" t="s">
         <v>24</v>
@@ -2483,10 +2480,10 @@
         <v>94</v>
       </c>
       <c r="C46" s="1">
-        <v>42459.333333333336</v>
+        <v>40997.333333333336</v>
       </c>
       <c r="D46" s="1">
-        <v>42459.708333333336</v>
+        <v>40997.708333333336</v>
       </c>
       <c r="E46" t="s">
         <v>24</v>
@@ -2509,10 +2506,10 @@
         <v>96</v>
       </c>
       <c r="C47" s="1">
-        <v>42517.333333333336</v>
+        <v>41055.333333333336</v>
       </c>
       <c r="D47" s="1">
-        <v>42517.708333333336</v>
+        <v>41055.708333333336</v>
       </c>
       <c r="E47" t="s">
         <v>24</v>
@@ -2524,7 +2521,7 @@
         <v>0</v>
       </c>
       <c r="N47" s="1">
-        <v>42517.333333333336</v>
+        <v>41055.333333333336</v>
       </c>
       <c r="R47">
         <v>0</v>
@@ -2538,10 +2535,10 @@
         <v>98</v>
       </c>
       <c r="C48" s="1">
-        <v>42517.333333333336</v>
+        <v>41055.333333333336</v>
       </c>
       <c r="D48" s="1">
-        <v>42517.708333333336</v>
+        <v>41055.708333333336</v>
       </c>
       <c r="E48" t="s">
         <v>24</v>
@@ -2553,7 +2550,7 @@
         <v>0</v>
       </c>
       <c r="N48" s="1">
-        <v>42517.333333333336</v>
+        <v>41055.333333333336</v>
       </c>
       <c r="R48">
         <v>0</v>
@@ -2567,10 +2564,10 @@
         <v>99</v>
       </c>
       <c r="C49" s="1">
-        <v>42459.333333333336</v>
+        <v>40997.333333333336</v>
       </c>
       <c r="D49" s="1">
-        <v>42517.708333333336</v>
+        <v>41055.708333333336</v>
       </c>
       <c r="E49" t="s">
         <v>21</v>
@@ -2590,10 +2587,10 @@
         <v>101</v>
       </c>
       <c r="C50" s="1">
-        <v>42459.333333333336</v>
+        <v>40997.333333333336</v>
       </c>
       <c r="D50" s="1">
-        <v>42459.708333333336</v>
+        <v>40997.708333333336</v>
       </c>
       <c r="E50" t="s">
         <v>24</v>
@@ -2616,10 +2613,10 @@
         <v>103</v>
       </c>
       <c r="C51" s="1">
-        <v>42459.333333333336</v>
+        <v>40997.333333333336</v>
       </c>
       <c r="D51" s="1">
-        <v>42459.708333333336</v>
+        <v>40997.708333333336</v>
       </c>
       <c r="E51" t="s">
         <v>24</v>
@@ -2642,10 +2639,10 @@
         <v>105</v>
       </c>
       <c r="C52" s="1">
-        <v>42517.333333333336</v>
+        <v>41055.333333333336</v>
       </c>
       <c r="D52" s="1">
-        <v>42517.708333333336</v>
+        <v>41055.708333333336</v>
       </c>
       <c r="E52" t="s">
         <v>24</v>
@@ -2657,7 +2654,7 @@
         <v>0</v>
       </c>
       <c r="N52" s="1">
-        <v>42517.333333333336</v>
+        <v>41055.333333333336</v>
       </c>
       <c r="R52">
         <v>0</v>
@@ -2671,10 +2668,10 @@
         <v>107</v>
       </c>
       <c r="C53" s="1">
-        <v>42517.333333333336</v>
+        <v>41055.333333333336</v>
       </c>
       <c r="D53" s="1">
-        <v>42517.708333333336</v>
+        <v>41055.708333333336</v>
       </c>
       <c r="E53" t="s">
         <v>24</v>
@@ -2686,7 +2683,7 @@
         <v>0</v>
       </c>
       <c r="N53" s="1">
-        <v>42517.333333333336</v>
+        <v>41055.333333333336</v>
       </c>
       <c r="R53">
         <v>0</v>
@@ -2700,10 +2697,10 @@
         <v>109</v>
       </c>
       <c r="C54" s="1">
-        <v>42517.333333333336</v>
+        <v>41055.333333333336</v>
       </c>
       <c r="D54" s="1">
-        <v>42517.708333333336</v>
+        <v>41055.708333333336</v>
       </c>
       <c r="E54" t="s">
         <v>24</v>
@@ -2715,7 +2712,7 @@
         <v>0</v>
       </c>
       <c r="N54" s="1">
-        <v>42517.333333333336</v>
+        <v>41055.333333333336</v>
       </c>
       <c r="R54">
         <v>0</v>
@@ -2729,10 +2726,10 @@
         <v>110</v>
       </c>
       <c r="C55" s="1">
-        <v>42459.333333333336</v>
+        <v>40997.333333333336</v>
       </c>
       <c r="D55" s="1">
-        <v>42459.708333333336</v>
+        <v>40997.708333333336</v>
       </c>
       <c r="E55" t="s">
         <v>24</v>
@@ -2752,10 +2749,10 @@
         <v>112</v>
       </c>
       <c r="C56" s="1">
-        <v>42459.333333333336</v>
+        <v>40997.333333333336</v>
       </c>
       <c r="D56" s="1">
-        <v>42459.708333333336</v>
+        <v>40997.708333333336</v>
       </c>
       <c r="E56" t="s">
         <v>24</v>
@@ -2778,10 +2775,10 @@
         <v>114</v>
       </c>
       <c r="C57" s="1">
-        <v>42459.333333333336</v>
+        <v>40997.333333333336</v>
       </c>
       <c r="D57" s="1">
-        <v>42459.708333333336</v>
+        <v>40997.708333333336</v>
       </c>
       <c r="E57" t="s">
         <v>24</v>
@@ -2804,10 +2801,10 @@
         <v>116</v>
       </c>
       <c r="C58" s="1">
-        <v>42459.333333333336</v>
+        <v>40997.333333333336</v>
       </c>
       <c r="D58" s="1">
-        <v>42459.708333333336</v>
+        <v>40997.708333333336</v>
       </c>
       <c r="E58" t="s">
         <v>24</v>
@@ -2830,10 +2827,10 @@
         <v>118</v>
       </c>
       <c r="C59" s="1">
-        <v>42459.333333333336</v>
+        <v>40997.333333333336</v>
       </c>
       <c r="D59" s="1">
-        <v>42459.708333333336</v>
+        <v>40997.708333333336</v>
       </c>
       <c r="E59" t="s">
         <v>24</v>
@@ -2856,10 +2853,10 @@
         <v>120</v>
       </c>
       <c r="C60" s="1">
-        <v>42459.333333333336</v>
+        <v>40997.333333333336</v>
       </c>
       <c r="D60" s="1">
-        <v>42459.708333333336</v>
+        <v>40997.708333333336</v>
       </c>
       <c r="E60" t="s">
         <v>24</v>
@@ -2882,10 +2879,10 @@
         <v>121</v>
       </c>
       <c r="C61" s="1">
-        <v>42461.333333333336</v>
+        <v>40999.333333333336</v>
       </c>
       <c r="D61" s="1">
-        <v>42517.708333333336</v>
+        <v>41055.708333333336</v>
       </c>
       <c r="E61" t="s">
         <v>38</v>
@@ -2897,7 +2894,7 @@
         <v>0</v>
       </c>
       <c r="N61" s="1">
-        <v>42461.333333333336</v>
+        <v>40999.333333333336</v>
       </c>
     </row>
     <row r="62" spans="1:18">
@@ -2908,10 +2905,10 @@
         <v>123</v>
       </c>
       <c r="C62" s="1">
-        <v>42461.333333333336</v>
+        <v>40999.333333333336</v>
       </c>
       <c r="D62" s="1">
-        <v>42461.708333333336</v>
+        <v>40999.708333333336</v>
       </c>
       <c r="E62" t="s">
         <v>24</v>
@@ -2931,10 +2928,10 @@
         <v>126</v>
       </c>
       <c r="C63" s="1">
-        <v>42461.333333333336</v>
+        <v>40999.333333333336</v>
       </c>
       <c r="D63" s="1">
-        <v>42461.708333333336</v>
+        <v>40999.708333333336</v>
       </c>
       <c r="E63" t="s">
         <v>24</v>
@@ -2957,10 +2954,10 @@
         <v>128</v>
       </c>
       <c r="C64" s="1">
-        <v>42461.333333333336</v>
+        <v>40999.333333333336</v>
       </c>
       <c r="D64" s="1">
-        <v>42461.708333333336</v>
+        <v>40999.708333333336</v>
       </c>
       <c r="E64" t="s">
         <v>24</v>
@@ -2983,10 +2980,10 @@
         <v>130</v>
       </c>
       <c r="C65" s="1">
-        <v>42461.333333333336</v>
+        <v>40999.333333333336</v>
       </c>
       <c r="D65" s="1">
-        <v>42461.708333333336</v>
+        <v>40999.708333333336</v>
       </c>
       <c r="E65" t="s">
         <v>24</v>
@@ -3009,10 +3006,10 @@
         <v>132</v>
       </c>
       <c r="C66" s="1">
-        <v>42461.333333333336</v>
+        <v>40999.333333333336</v>
       </c>
       <c r="D66" s="1">
-        <v>42461.708333333336</v>
+        <v>40999.708333333336</v>
       </c>
       <c r="E66" t="s">
         <v>24</v>
@@ -3035,10 +3032,10 @@
         <v>133</v>
       </c>
       <c r="C67" s="1">
-        <v>42461.333333333336</v>
+        <v>40999.333333333336</v>
       </c>
       <c r="D67" s="1">
-        <v>42461.708333333336</v>
+        <v>40999.708333333336</v>
       </c>
       <c r="E67" t="s">
         <v>24</v>
@@ -3058,10 +3055,10 @@
         <v>135</v>
       </c>
       <c r="C68" s="1">
-        <v>42461.333333333336</v>
+        <v>40999.333333333336</v>
       </c>
       <c r="D68" s="1">
-        <v>42461.708333333336</v>
+        <v>40999.708333333336</v>
       </c>
       <c r="E68" t="s">
         <v>24</v>
@@ -3084,10 +3081,10 @@
         <v>137</v>
       </c>
       <c r="C69" s="1">
-        <v>42461.333333333336</v>
+        <v>40999.333333333336</v>
       </c>
       <c r="D69" s="1">
-        <v>42461.708333333336</v>
+        <v>40999.708333333336</v>
       </c>
       <c r="E69" t="s">
         <v>24</v>
@@ -3110,10 +3107,10 @@
         <v>139</v>
       </c>
       <c r="C70" s="1">
-        <v>42461.333333333336</v>
+        <v>40999.333333333336</v>
       </c>
       <c r="D70" s="1">
-        <v>42461.708333333336</v>
+        <v>40999.708333333336</v>
       </c>
       <c r="E70" t="s">
         <v>24</v>
@@ -3136,10 +3133,10 @@
         <v>141</v>
       </c>
       <c r="C71" s="1">
-        <v>42461.333333333336</v>
+        <v>40999.333333333336</v>
       </c>
       <c r="D71" s="1">
-        <v>42461.708333333336</v>
+        <v>40999.708333333336</v>
       </c>
       <c r="E71" t="s">
         <v>24</v>
@@ -3162,10 +3159,10 @@
         <v>142</v>
       </c>
       <c r="C72" s="1">
-        <v>42461.333333333336</v>
+        <v>40999.333333333336</v>
       </c>
       <c r="D72" s="1">
-        <v>42461.708333333336</v>
+        <v>40999.708333333336</v>
       </c>
       <c r="E72" t="s">
         <v>24</v>
@@ -3177,7 +3174,7 @@
         <v>0</v>
       </c>
       <c r="N72" s="1">
-        <v>42461.333333333336</v>
+        <v>40999.333333333336</v>
       </c>
     </row>
     <row r="73" spans="1:18">
@@ -3188,10 +3185,10 @@
         <v>144</v>
       </c>
       <c r="C73" s="1">
-        <v>42461.333333333336</v>
+        <v>40999.333333333336</v>
       </c>
       <c r="D73" s="1">
-        <v>42461.708333333336</v>
+        <v>40999.708333333336</v>
       </c>
       <c r="E73" t="s">
         <v>24</v>
@@ -3214,10 +3211,10 @@
         <v>146</v>
       </c>
       <c r="C74" s="1">
-        <v>42461.333333333336</v>
+        <v>40999.333333333336</v>
       </c>
       <c r="D74" s="1">
-        <v>42461.708333333336</v>
+        <v>40999.708333333336</v>
       </c>
       <c r="E74" t="s">
         <v>24</v>
@@ -3240,10 +3237,10 @@
         <v>148</v>
       </c>
       <c r="C75" s="1">
-        <v>42461.333333333336</v>
+        <v>40999.333333333336</v>
       </c>
       <c r="D75" s="1">
-        <v>42461.708333333336</v>
+        <v>40999.708333333336</v>
       </c>
       <c r="E75" t="s">
         <v>24</v>
@@ -3266,10 +3263,10 @@
         <v>150</v>
       </c>
       <c r="C76" s="1">
-        <v>42461.333333333336</v>
+        <v>40999.333333333336</v>
       </c>
       <c r="D76" s="1">
-        <v>42461.708333333336</v>
+        <v>40999.708333333336</v>
       </c>
       <c r="E76" t="s">
         <v>24</v>
@@ -3292,10 +3289,10 @@
         <v>151</v>
       </c>
       <c r="C77" s="1">
-        <v>42517.333333333336</v>
+        <v>41055.333333333336</v>
       </c>
       <c r="D77" s="1">
-        <v>42517.708333333336</v>
+        <v>41055.708333333336</v>
       </c>
       <c r="E77" t="s">
         <v>24</v>
@@ -3307,7 +3304,7 @@
         <v>0</v>
       </c>
       <c r="N77" s="1">
-        <v>42517.333333333336</v>
+        <v>41055.333333333336</v>
       </c>
     </row>
     <row r="78" spans="1:18">
@@ -3318,10 +3315,10 @@
         <v>153</v>
       </c>
       <c r="C78" s="1">
-        <v>42517.333333333336</v>
+        <v>41055.333333333336</v>
       </c>
       <c r="D78" s="1">
-        <v>42517.708333333336</v>
+        <v>41055.708333333336</v>
       </c>
       <c r="E78" t="s">
         <v>24</v>
@@ -3333,7 +3330,7 @@
         <v>0</v>
       </c>
       <c r="N78" s="1">
-        <v>42517.333333333336</v>
+        <v>41055.333333333336</v>
       </c>
       <c r="R78">
         <v>0</v>
@@ -3347,10 +3344,10 @@
         <v>155</v>
       </c>
       <c r="C79" s="1">
-        <v>42517.333333333336</v>
+        <v>41055.333333333336</v>
       </c>
       <c r="D79" s="1">
-        <v>42517.708333333336</v>
+        <v>41055.708333333336</v>
       </c>
       <c r="E79" t="s">
         <v>24</v>
@@ -3362,7 +3359,7 @@
         <v>0</v>
       </c>
       <c r="N79" s="1">
-        <v>42517.333333333336</v>
+        <v>41055.333333333336</v>
       </c>
       <c r="R79">
         <v>0</v>
@@ -3376,10 +3373,10 @@
         <v>157</v>
       </c>
       <c r="C80" s="1">
-        <v>42517.333333333336</v>
+        <v>41055.333333333336</v>
       </c>
       <c r="D80" s="1">
-        <v>42517.708333333336</v>
+        <v>41055.708333333336</v>
       </c>
       <c r="E80" t="s">
         <v>24</v>
@@ -3391,7 +3388,7 @@
         <v>0</v>
       </c>
       <c r="N80" s="1">
-        <v>42517.333333333336</v>
+        <v>41055.333333333336</v>
       </c>
       <c r="R80">
         <v>0</v>
@@ -3405,10 +3402,10 @@
         <v>159</v>
       </c>
       <c r="C81" s="1">
-        <v>42517.333333333336</v>
+        <v>41055.333333333336</v>
       </c>
       <c r="D81" s="1">
-        <v>42517.708333333336</v>
+        <v>41055.708333333336</v>
       </c>
       <c r="E81" t="s">
         <v>24</v>
@@ -3420,7 +3417,7 @@
         <v>0</v>
       </c>
       <c r="N81" s="1">
-        <v>42517.333333333336</v>
+        <v>41055.333333333336</v>
       </c>
       <c r="R81">
         <v>0</v>
@@ -3434,10 +3431,10 @@
         <v>160</v>
       </c>
       <c r="C82" s="1">
-        <v>42461.333333333336</v>
+        <v>40999.333333333336</v>
       </c>
       <c r="D82" s="1">
-        <v>42461.708333333336</v>
+        <v>40999.708333333336</v>
       </c>
       <c r="E82" t="s">
         <v>24</v>
@@ -3457,10 +3454,10 @@
         <v>162</v>
       </c>
       <c r="C83" s="1">
-        <v>42461.333333333336</v>
+        <v>40999.333333333336</v>
       </c>
       <c r="D83" s="1">
-        <v>42461.708333333336</v>
+        <v>40999.708333333336</v>
       </c>
       <c r="E83" t="s">
         <v>24</v>
@@ -3483,10 +3480,10 @@
         <v>164</v>
       </c>
       <c r="C84" s="1">
-        <v>42461.333333333336</v>
+        <v>40999.333333333336</v>
       </c>
       <c r="D84" s="1">
-        <v>42461.708333333336</v>
+        <v>40999.708333333336</v>
       </c>
       <c r="E84" t="s">
         <v>24</v>
@@ -3509,10 +3506,10 @@
         <v>166</v>
       </c>
       <c r="C85" s="1">
-        <v>42461.333333333336</v>
+        <v>40999.333333333336</v>
       </c>
       <c r="D85" s="1">
-        <v>42461.708333333336</v>
+        <v>40999.708333333336</v>
       </c>
       <c r="E85" t="s">
         <v>24</v>
@@ -3535,10 +3532,10 @@
         <v>168</v>
       </c>
       <c r="C86" s="1">
-        <v>42461.333333333336</v>
+        <v>40999.333333333336</v>
       </c>
       <c r="D86" s="1">
-        <v>42461.708333333336</v>
+        <v>40999.708333333336</v>
       </c>
       <c r="E86" t="s">
         <v>24</v>
@@ -3561,10 +3558,10 @@
         <v>170</v>
       </c>
       <c r="C87" s="1">
-        <v>42461.333333333336</v>
+        <v>40999.333333333336</v>
       </c>
       <c r="D87" s="1">
-        <v>42461.708333333336</v>
+        <v>40999.708333333336</v>
       </c>
       <c r="E87" t="s">
         <v>24</v>
@@ -3587,10 +3584,10 @@
         <v>172</v>
       </c>
       <c r="C88" s="1">
-        <v>42461.333333333336</v>
+        <v>40999.333333333336</v>
       </c>
       <c r="D88" s="1">
-        <v>42461.708333333336</v>
+        <v>40999.708333333336</v>
       </c>
       <c r="E88" t="s">
         <v>24</v>
@@ -3613,10 +3610,10 @@
         <v>173</v>
       </c>
       <c r="C89" s="1">
-        <v>42461.333333333336</v>
+        <v>40999.333333333336</v>
       </c>
       <c r="D89" s="1">
-        <v>42461.708333333336</v>
+        <v>40999.708333333336</v>
       </c>
       <c r="E89" t="s">
         <v>24</v>
@@ -3636,10 +3633,10 @@
         <v>176</v>
       </c>
       <c r="C90" s="1">
-        <v>42461.333333333336</v>
+        <v>40999.333333333336</v>
       </c>
       <c r="D90" s="1">
-        <v>42461.708333333336</v>
+        <v>40999.708333333336</v>
       </c>
       <c r="E90" t="s">
         <v>24</v>
@@ -3662,10 +3659,10 @@
         <v>178</v>
       </c>
       <c r="C91" s="1">
-        <v>42461.333333333336</v>
+        <v>40999.333333333336</v>
       </c>
       <c r="D91" s="1">
-        <v>42461.708333333336</v>
+        <v>40999.708333333336</v>
       </c>
       <c r="E91" t="s">
         <v>24</v>
@@ -3688,10 +3685,10 @@
         <v>180</v>
       </c>
       <c r="C92" s="1">
-        <v>42461.333333333336</v>
+        <v>40999.333333333336</v>
       </c>
       <c r="D92" s="1">
-        <v>42461.708333333336</v>
+        <v>40999.708333333336</v>
       </c>
       <c r="E92" t="s">
         <v>24</v>
@@ -3714,10 +3711,10 @@
         <v>182</v>
       </c>
       <c r="C93" s="1">
-        <v>42461.333333333336</v>
+        <v>40999.333333333336</v>
       </c>
       <c r="D93" s="1">
-        <v>42461.708333333336</v>
+        <v>40999.708333333336</v>
       </c>
       <c r="E93" t="s">
         <v>24</v>
@@ -3737,10 +3734,10 @@
         <v>184</v>
       </c>
       <c r="C94" s="1">
-        <v>42461.333333333336</v>
+        <v>40999.333333333336</v>
       </c>
       <c r="D94" s="1">
-        <v>42461.708333333336</v>
+        <v>40999.708333333336</v>
       </c>
       <c r="E94" t="s">
         <v>24</v>
@@ -3763,10 +3760,10 @@
         <v>186</v>
       </c>
       <c r="C95" s="1">
-        <v>42461.333333333336</v>
+        <v>40999.333333333336</v>
       </c>
       <c r="D95" s="1">
-        <v>42461.708333333336</v>
+        <v>40999.708333333336</v>
       </c>
       <c r="E95" t="s">
         <v>24</v>
@@ -3789,10 +3786,10 @@
         <v>188</v>
       </c>
       <c r="C96" s="1">
-        <v>42461.333333333336</v>
+        <v>40999.333333333336</v>
       </c>
       <c r="D96" s="1">
-        <v>42461.708333333336</v>
+        <v>40999.708333333336</v>
       </c>
       <c r="E96" t="s">
         <v>24</v>
@@ -3815,10 +3812,10 @@
         <v>190</v>
       </c>
       <c r="C97" s="1">
-        <v>42461.333333333336</v>
+        <v>40999.333333333336</v>
       </c>
       <c r="D97" s="1">
-        <v>42461.708333333336</v>
+        <v>40999.708333333336</v>
       </c>
       <c r="E97" t="s">
         <v>24</v>
@@ -3841,10 +3838,10 @@
         <v>192</v>
       </c>
       <c r="C98" s="1">
-        <v>42461.333333333336</v>
+        <v>40999.333333333336</v>
       </c>
       <c r="D98" s="1">
-        <v>42461.708333333336</v>
+        <v>40999.708333333336</v>
       </c>
       <c r="E98" t="s">
         <v>24</v>
@@ -3867,10 +3864,10 @@
         <v>194</v>
       </c>
       <c r="C99" s="1">
-        <v>42461.333333333336</v>
+        <v>40999.333333333336</v>
       </c>
       <c r="D99" s="1">
-        <v>42461.708333333336</v>
+        <v>40999.708333333336</v>
       </c>
       <c r="E99" t="s">
         <v>24</v>
@@ -3893,10 +3890,10 @@
         <v>196</v>
       </c>
       <c r="C100" s="1">
-        <v>42461.333333333336</v>
+        <v>40999.333333333336</v>
       </c>
       <c r="D100" s="1">
-        <v>42461.708333333336</v>
+        <v>40999.708333333336</v>
       </c>
       <c r="E100" t="s">
         <v>24</v>
@@ -3919,10 +3916,10 @@
         <v>198</v>
       </c>
       <c r="C101" s="1">
-        <v>42461.333333333336</v>
+        <v>40999.333333333336</v>
       </c>
       <c r="D101" s="1">
-        <v>42461.708333333336</v>
+        <v>40999.708333333336</v>
       </c>
       <c r="E101" t="s">
         <v>24</v>
@@ -3945,10 +3942,10 @@
         <v>200</v>
       </c>
       <c r="C102" s="1">
-        <v>42461.333333333336</v>
+        <v>40999.333333333336</v>
       </c>
       <c r="D102" s="1">
-        <v>42461.708333333336</v>
+        <v>40999.708333333336</v>
       </c>
       <c r="E102" t="s">
         <v>24</v>
@@ -3971,10 +3968,10 @@
         <v>202</v>
       </c>
       <c r="C103" s="1">
-        <v>42461.333333333336</v>
+        <v>40999.333333333336</v>
       </c>
       <c r="D103" s="1">
-        <v>42461.708333333336</v>
+        <v>40999.708333333336</v>
       </c>
       <c r="E103" t="s">
         <v>24</v>
@@ -3997,10 +3994,10 @@
         <v>204</v>
       </c>
       <c r="C104" s="1">
-        <v>42461.333333333336</v>
+        <v>40999.333333333336</v>
       </c>
       <c r="D104" s="1">
-        <v>42461.708333333336</v>
+        <v>40999.708333333336</v>
       </c>
       <c r="E104" t="s">
         <v>24</v>
@@ -4023,10 +4020,10 @@
         <v>205</v>
       </c>
       <c r="C105" s="1">
-        <v>42461.333333333336</v>
+        <v>40999.333333333336</v>
       </c>
       <c r="D105" s="1">
-        <v>42461.708333333336</v>
+        <v>40999.708333333336</v>
       </c>
       <c r="E105" t="s">
         <v>24</v>
@@ -4046,10 +4043,10 @@
         <v>207</v>
       </c>
       <c r="C106" s="1">
-        <v>42461.333333333336</v>
+        <v>40999.333333333336</v>
       </c>
       <c r="D106" s="1">
-        <v>42461.708333333336</v>
+        <v>40999.708333333336</v>
       </c>
       <c r="E106" t="s">
         <v>24</v>
@@ -4072,10 +4069,10 @@
         <v>209</v>
       </c>
       <c r="C107" s="1">
-        <v>42461.333333333336</v>
+        <v>40999.333333333336</v>
       </c>
       <c r="D107" s="1">
-        <v>42461.708333333336</v>
+        <v>40999.708333333336</v>
       </c>
       <c r="E107" t="s">
         <v>24</v>
@@ -4098,10 +4095,10 @@
         <v>211</v>
       </c>
       <c r="C108" s="1">
-        <v>42461.333333333336</v>
+        <v>40999.333333333336</v>
       </c>
       <c r="D108" s="1">
-        <v>42461.708333333336</v>
+        <v>40999.708333333336</v>
       </c>
       <c r="E108" t="s">
         <v>24</v>
@@ -4124,10 +4121,10 @@
         <v>213</v>
       </c>
       <c r="C109" s="1">
-        <v>42461.333333333336</v>
+        <v>40999.333333333336</v>
       </c>
       <c r="D109" s="1">
-        <v>42461.708333333336</v>
+        <v>40999.708333333336</v>
       </c>
       <c r="E109" t="s">
         <v>24</v>
@@ -4150,10 +4147,10 @@
         <v>215</v>
       </c>
       <c r="C110" s="1">
-        <v>42461.333333333336</v>
+        <v>40999.333333333336</v>
       </c>
       <c r="D110" s="1">
-        <v>42461.708333333336</v>
+        <v>40999.708333333336</v>
       </c>
       <c r="E110" t="s">
         <v>24</v>
@@ -4176,10 +4173,10 @@
         <v>217</v>
       </c>
       <c r="C111" s="1">
-        <v>42461.333333333336</v>
+        <v>40999.333333333336</v>
       </c>
       <c r="D111" s="1">
-        <v>42461.708333333336</v>
+        <v>40999.708333333336</v>
       </c>
       <c r="E111" t="s">
         <v>24</v>
@@ -4202,10 +4199,10 @@
         <v>218</v>
       </c>
       <c r="C112" s="1">
-        <v>42461.333333333336</v>
+        <v>40999.333333333336</v>
       </c>
       <c r="D112" s="1">
-        <v>42517.708333333336</v>
+        <v>41055.708333333336</v>
       </c>
       <c r="E112" t="s">
         <v>38</v>
@@ -4217,7 +4214,7 @@
         <v>0</v>
       </c>
       <c r="N112" s="1">
-        <v>42461.333333333336</v>
+        <v>40999.333333333336</v>
       </c>
     </row>
     <row r="113" spans="1:18">
@@ -4228,10 +4225,10 @@
         <v>219</v>
       </c>
       <c r="C113" s="1">
-        <v>42517.333333333336</v>
+        <v>41055.333333333336</v>
       </c>
       <c r="D113" s="1">
-        <v>42517.708333333336</v>
+        <v>41055.708333333336</v>
       </c>
       <c r="E113" t="s">
         <v>24</v>
@@ -4243,7 +4240,7 @@
         <v>0</v>
       </c>
       <c r="N113" s="1">
-        <v>42517.333333333336</v>
+        <v>41055.333333333336</v>
       </c>
       <c r="R113">
         <v>0</v>
@@ -4257,10 +4254,10 @@
         <v>220</v>
       </c>
       <c r="C114" s="1">
-        <v>42517.333333333336</v>
+        <v>41055.333333333336</v>
       </c>
       <c r="D114" s="1">
-        <v>42517.708333333336</v>
+        <v>41055.708333333336</v>
       </c>
       <c r="E114" t="s">
         <v>24</v>
@@ -4272,7 +4269,7 @@
         <v>0</v>
       </c>
       <c r="N114" s="1">
-        <v>42517.333333333336</v>
+        <v>41055.333333333336</v>
       </c>
       <c r="R114">
         <v>0</v>
@@ -4286,10 +4283,10 @@
         <v>221</v>
       </c>
       <c r="C115" s="1">
-        <v>42461.333333333336</v>
+        <v>40999.333333333336</v>
       </c>
       <c r="D115" s="1">
-        <v>42461.708333333336</v>
+        <v>40999.708333333336</v>
       </c>
       <c r="E115" t="s">
         <v>24</v>
@@ -4312,10 +4309,10 @@
         <v>222</v>
       </c>
       <c r="C116" s="1">
-        <v>42461.333333333336</v>
+        <v>40999.333333333336</v>
       </c>
       <c r="D116" s="1">
-        <v>42461.708333333336</v>
+        <v>40999.708333333336</v>
       </c>
       <c r="E116" t="s">
         <v>24</v>
@@ -4338,10 +4335,10 @@
         <v>223</v>
       </c>
       <c r="C117" s="1">
-        <v>42461.333333333336</v>
+        <v>40999.333333333336</v>
       </c>
       <c r="D117" s="1">
-        <v>42461.708333333336</v>
+        <v>40999.708333333336</v>
       </c>
       <c r="E117" t="s">
         <v>24</v>
@@ -4364,10 +4361,10 @@
         <v>224</v>
       </c>
       <c r="C118" s="1">
-        <v>42461.333333333336</v>
+        <v>40999.333333333336</v>
       </c>
       <c r="D118" s="1">
-        <v>42461.708333333336</v>
+        <v>40999.708333333336</v>
       </c>
       <c r="E118" t="s">
         <v>24</v>
@@ -4390,10 +4387,10 @@
         <v>225</v>
       </c>
       <c r="C119" s="1">
-        <v>42517.333333333336</v>
+        <v>41055.333333333336</v>
       </c>
       <c r="D119" s="1">
-        <v>42517.708333333336</v>
+        <v>41055.708333333336</v>
       </c>
       <c r="E119" t="s">
         <v>24</v>
@@ -4405,7 +4402,7 @@
         <v>0</v>
       </c>
       <c r="N119" s="1">
-        <v>42461.333333333336</v>
+        <v>40999.333333333336</v>
       </c>
     </row>
     <row r="120" spans="1:18">
@@ -4416,10 +4413,10 @@
         <v>226</v>
       </c>
       <c r="C120" s="1">
-        <v>42517.333333333336</v>
+        <v>41055.333333333336</v>
       </c>
       <c r="D120" s="1">
-        <v>42517.708333333336</v>
+        <v>41055.708333333336</v>
       </c>
       <c r="E120" t="s">
         <v>24</v>
@@ -4431,7 +4428,7 @@
         <v>0</v>
       </c>
       <c r="N120" s="1">
-        <v>42517.333333333336</v>
+        <v>41055.333333333336</v>
       </c>
       <c r="R120">
         <v>0</v>
@@ -4445,10 +4442,10 @@
         <v>227</v>
       </c>
       <c r="C121" s="1">
-        <v>42517.333333333336</v>
+        <v>41055.333333333336</v>
       </c>
       <c r="D121" s="1">
-        <v>42517.708333333336</v>
+        <v>41055.708333333336</v>
       </c>
       <c r="E121" t="s">
         <v>24</v>
@@ -4460,7 +4457,7 @@
         <v>0</v>
       </c>
       <c r="N121" s="1">
-        <v>42517.333333333336</v>
+        <v>41055.333333333336</v>
       </c>
       <c r="R121">
         <v>0</v>
@@ -4474,10 +4471,10 @@
         <v>228</v>
       </c>
       <c r="C122" s="1">
-        <v>42517.333333333336</v>
+        <v>41055.333333333336</v>
       </c>
       <c r="D122" s="1">
-        <v>42517.708333333336</v>
+        <v>41055.708333333336</v>
       </c>
       <c r="E122" t="s">
         <v>24</v>
@@ -4489,7 +4486,7 @@
         <v>0</v>
       </c>
       <c r="N122" s="1">
-        <v>42517.333333333336</v>
+        <v>41055.333333333336</v>
       </c>
       <c r="R122">
         <v>0</v>
@@ -4503,10 +4500,10 @@
         <v>229</v>
       </c>
       <c r="C123" s="1">
-        <v>42517.333333333336</v>
+        <v>41055.333333333336</v>
       </c>
       <c r="D123" s="1">
-        <v>42517.708333333336</v>
+        <v>41055.708333333336</v>
       </c>
       <c r="E123" t="s">
         <v>24</v>
@@ -4518,7 +4515,7 @@
         <v>0</v>
       </c>
       <c r="N123" s="1">
-        <v>42517.333333333336</v>
+        <v>41055.333333333336</v>
       </c>
       <c r="R123">
         <v>0</v>
@@ -4532,10 +4529,10 @@
         <v>230</v>
       </c>
       <c r="C124" s="1">
-        <v>42517.333333333336</v>
+        <v>41055.333333333336</v>
       </c>
       <c r="D124" s="1">
-        <v>42517.708333333336</v>
+        <v>41055.708333333336</v>
       </c>
       <c r="E124" t="s">
         <v>24</v>
@@ -4547,7 +4544,7 @@
         <v>0</v>
       </c>
       <c r="N124" s="1">
-        <v>42517.333333333336</v>
+        <v>41055.333333333336</v>
       </c>
       <c r="R124">
         <v>0</v>
@@ -4561,10 +4558,10 @@
         <v>231</v>
       </c>
       <c r="C125" s="1">
-        <v>42517.333333333336</v>
+        <v>41055.333333333336</v>
       </c>
       <c r="D125" s="1">
-        <v>42517.708333333336</v>
+        <v>41055.708333333336</v>
       </c>
       <c r="E125" t="s">
         <v>24</v>
@@ -4576,7 +4573,7 @@
         <v>0</v>
       </c>
       <c r="N125" s="1">
-        <v>42517.333333333336</v>
+        <v>41055.333333333336</v>
       </c>
       <c r="R125">
         <v>0</v>
@@ -4590,10 +4587,10 @@
         <v>232</v>
       </c>
       <c r="C126" s="1">
-        <v>42517.333333333336</v>
+        <v>41055.333333333336</v>
       </c>
       <c r="D126" s="1">
-        <v>42517.708333333336</v>
+        <v>41055.708333333336</v>
       </c>
       <c r="E126" t="s">
         <v>24</v>
@@ -4605,7 +4602,7 @@
         <v>0</v>
       </c>
       <c r="N126" s="1">
-        <v>42517.333333333336</v>
+        <v>41055.333333333336</v>
       </c>
       <c r="R126">
         <v>0</v>
@@ -4619,10 +4616,10 @@
         <v>233</v>
       </c>
       <c r="C127" s="1">
-        <v>42517.333333333336</v>
+        <v>41055.333333333336</v>
       </c>
       <c r="D127" s="1">
-        <v>42517.708333333336</v>
+        <v>41055.708333333336</v>
       </c>
       <c r="E127" t="s">
         <v>24</v>
@@ -4634,7 +4631,7 @@
         <v>0</v>
       </c>
       <c r="N127" s="1">
-        <v>42517.333333333336</v>
+        <v>41055.333333333336</v>
       </c>
       <c r="R127">
         <v>0</v>
@@ -4648,10 +4645,10 @@
         <v>234</v>
       </c>
       <c r="C128" s="1">
-        <v>42517.333333333336</v>
+        <v>41055.333333333336</v>
       </c>
       <c r="D128" s="1">
-        <v>42517.708333333336</v>
+        <v>41055.708333333336</v>
       </c>
       <c r="E128" t="s">
         <v>24</v>
@@ -4663,7 +4660,7 @@
         <v>0</v>
       </c>
       <c r="N128" s="1">
-        <v>42517.333333333336</v>
+        <v>41055.333333333336</v>
       </c>
       <c r="R128">
         <v>0</v>
@@ -4677,10 +4674,10 @@
         <v>235</v>
       </c>
       <c r="C129" s="1">
-        <v>42461.333333333336</v>
+        <v>40999.333333333336</v>
       </c>
       <c r="D129" s="1">
-        <v>42517.708333333336</v>
+        <v>41055.708333333336</v>
       </c>
       <c r="E129" t="s">
         <v>38</v>
@@ -4692,7 +4689,7 @@
         <v>0</v>
       </c>
       <c r="N129" s="1">
-        <v>42461.333333333336</v>
+        <v>40999.333333333336</v>
       </c>
     </row>
     <row r="130" spans="1:18">
@@ -4703,10 +4700,10 @@
         <v>236</v>
       </c>
       <c r="C130" s="1">
-        <v>42461.333333333336</v>
+        <v>40999.333333333336</v>
       </c>
       <c r="D130" s="1">
-        <v>42461.708333333336</v>
+        <v>40999.708333333336</v>
       </c>
       <c r="E130" t="s">
         <v>24</v>
@@ -4729,10 +4726,10 @@
         <v>237</v>
       </c>
       <c r="C131" s="1">
-        <v>42461.333333333336</v>
+        <v>40999.333333333336</v>
       </c>
       <c r="D131" s="1">
-        <v>42461.708333333336</v>
+        <v>40999.708333333336</v>
       </c>
       <c r="E131" t="s">
         <v>24</v>
@@ -4755,10 +4752,10 @@
         <v>238</v>
       </c>
       <c r="C132" s="1">
-        <v>42461.333333333336</v>
+        <v>40999.333333333336</v>
       </c>
       <c r="D132" s="1">
-        <v>42461.333333333336</v>
+        <v>40999.333333333336</v>
       </c>
       <c r="E132" t="s">
         <v>239</v>
@@ -4781,10 +4778,10 @@
         <v>240</v>
       </c>
       <c r="C133" s="1">
-        <v>42517.333333333336</v>
+        <v>41055.333333333336</v>
       </c>
       <c r="D133" s="1">
-        <v>42517.708333333336</v>
+        <v>41055.708333333336</v>
       </c>
       <c r="E133" t="s">
         <v>24</v>
@@ -4796,7 +4793,7 @@
         <v>0</v>
       </c>
       <c r="N133" s="1">
-        <v>42517.333333333336</v>
+        <v>41055.333333333336</v>
       </c>
       <c r="R133">
         <v>0</v>
@@ -4810,10 +4807,10 @@
         <v>241</v>
       </c>
       <c r="C134" s="1">
-        <v>42517.333333333336</v>
+        <v>41055.333333333336</v>
       </c>
       <c r="D134" s="1">
-        <v>42517.708333333336</v>
+        <v>41055.708333333336</v>
       </c>
       <c r="E134" t="s">
         <v>24</v>
@@ -4825,7 +4822,7 @@
         <v>0</v>
       </c>
       <c r="N134" s="1">
-        <v>42517.333333333336</v>
+        <v>41055.333333333336</v>
       </c>
       <c r="R134">
         <v>0</v>
@@ -4839,10 +4836,10 @@
         <v>242</v>
       </c>
       <c r="C135" s="1">
-        <v>42517.333333333336</v>
+        <v>41055.333333333336</v>
       </c>
       <c r="D135" s="1">
-        <v>42517.708333333336</v>
+        <v>41055.708333333336</v>
       </c>
       <c r="E135" t="s">
         <v>24</v>
@@ -4854,7 +4851,7 @@
         <v>0</v>
       </c>
       <c r="N135" s="1">
-        <v>42461.333333333336</v>
+        <v>40999.333333333336</v>
       </c>
     </row>
     <row r="136" spans="1:18">
@@ -4865,10 +4862,10 @@
         <v>244</v>
       </c>
       <c r="C136" s="1">
-        <v>42517.333333333336</v>
+        <v>41055.333333333336</v>
       </c>
       <c r="D136" s="1">
-        <v>42517.708333333336</v>
+        <v>41055.708333333336</v>
       </c>
       <c r="E136" t="s">
         <v>24</v>
@@ -4880,7 +4877,7 @@
         <v>0</v>
       </c>
       <c r="N136" s="1">
-        <v>42517.333333333336</v>
+        <v>41055.333333333336</v>
       </c>
     </row>
     <row r="137" spans="1:18">
@@ -4891,10 +4888,10 @@
         <v>246</v>
       </c>
       <c r="C137" s="1">
-        <v>42517.333333333336</v>
+        <v>41055.333333333336</v>
       </c>
       <c r="D137" s="1">
-        <v>42517.708333333336</v>
+        <v>41055.708333333336</v>
       </c>
       <c r="E137" t="s">
         <v>24</v>
@@ -4906,7 +4903,7 @@
         <v>0</v>
       </c>
       <c r="N137" s="1">
-        <v>42517.333333333336</v>
+        <v>41055.333333333336</v>
       </c>
       <c r="R137">
         <v>0</v>
@@ -4920,10 +4917,10 @@
         <v>248</v>
       </c>
       <c r="C138" s="1">
-        <v>42517.333333333336</v>
+        <v>41055.333333333336</v>
       </c>
       <c r="D138" s="1">
-        <v>42517.708333333336</v>
+        <v>41055.708333333336</v>
       </c>
       <c r="E138" t="s">
         <v>24</v>
@@ -4935,7 +4932,7 @@
         <v>0</v>
       </c>
       <c r="N138" s="1">
-        <v>42517.333333333336</v>
+        <v>41055.333333333336</v>
       </c>
       <c r="R138">
         <v>0</v>
@@ -4949,10 +4946,10 @@
         <v>250</v>
       </c>
       <c r="C139" s="1">
-        <v>42517.333333333336</v>
+        <v>41055.333333333336</v>
       </c>
       <c r="D139" s="1">
-        <v>42517.708333333336</v>
+        <v>41055.708333333336</v>
       </c>
       <c r="E139" t="s">
         <v>24</v>
@@ -4964,7 +4961,7 @@
         <v>0</v>
       </c>
       <c r="N139" s="1">
-        <v>42517.333333333336</v>
+        <v>41055.333333333336</v>
       </c>
       <c r="R139">
         <v>0</v>
@@ -4978,10 +4975,10 @@
         <v>252</v>
       </c>
       <c r="C140" s="1">
-        <v>42517.333333333336</v>
+        <v>41055.333333333336</v>
       </c>
       <c r="D140" s="1">
-        <v>42517.708333333336</v>
+        <v>41055.708333333336</v>
       </c>
       <c r="E140" t="s">
         <v>24</v>
@@ -5004,10 +5001,10 @@
         <v>253</v>
       </c>
       <c r="C141" s="1">
-        <v>42517.333333333336</v>
+        <v>41055.333333333336</v>
       </c>
       <c r="D141" s="1">
-        <v>42517.708333333336</v>
+        <v>41055.708333333336</v>
       </c>
       <c r="E141" t="s">
         <v>24</v>
@@ -5019,7 +5016,7 @@
         <v>0</v>
       </c>
       <c r="N141" s="1">
-        <v>42517.333333333336</v>
+        <v>41055.333333333336</v>
       </c>
     </row>
     <row r="142" spans="1:18">
@@ -5030,10 +5027,10 @@
         <v>255</v>
       </c>
       <c r="C142" s="1">
-        <v>42517.333333333336</v>
+        <v>41055.333333333336</v>
       </c>
       <c r="D142" s="1">
-        <v>42517.708333333336</v>
+        <v>41055.708333333336</v>
       </c>
       <c r="E142" t="s">
         <v>24</v>
@@ -5045,7 +5042,7 @@
         <v>0</v>
       </c>
       <c r="N142" s="1">
-        <v>42517.333333333336</v>
+        <v>41055.333333333336</v>
       </c>
       <c r="R142">
         <v>0</v>
@@ -5059,10 +5056,10 @@
         <v>257</v>
       </c>
       <c r="C143" s="1">
-        <v>42517.333333333336</v>
+        <v>41055.333333333336</v>
       </c>
       <c r="D143" s="1">
-        <v>42517.708333333336</v>
+        <v>41055.708333333336</v>
       </c>
       <c r="E143" t="s">
         <v>24</v>
@@ -5074,7 +5071,7 @@
         <v>0</v>
       </c>
       <c r="N143" s="1">
-        <v>42517.333333333336</v>
+        <v>41055.333333333336</v>
       </c>
       <c r="R143">
         <v>0</v>
@@ -5088,10 +5085,10 @@
         <v>259</v>
       </c>
       <c r="C144" s="1">
-        <v>42517.333333333336</v>
+        <v>41055.333333333336</v>
       </c>
       <c r="D144" s="1">
-        <v>42517.708333333336</v>
+        <v>41055.708333333336</v>
       </c>
       <c r="E144" t="s">
         <v>24</v>
@@ -5103,7 +5100,7 @@
         <v>0</v>
       </c>
       <c r="N144" s="1">
-        <v>42517.333333333336</v>
+        <v>41055.333333333336</v>
       </c>
       <c r="R144">
         <v>0</v>
@@ -5117,10 +5114,10 @@
         <v>261</v>
       </c>
       <c r="C145" s="1">
-        <v>42517.333333333336</v>
+        <v>41055.333333333336</v>
       </c>
       <c r="D145" s="1">
-        <v>42517.708333333336</v>
+        <v>41055.708333333336</v>
       </c>
       <c r="E145" t="s">
         <v>24</v>
@@ -5132,7 +5129,7 @@
         <v>0</v>
       </c>
       <c r="N145" s="1">
-        <v>42517.333333333336</v>
+        <v>41055.333333333336</v>
       </c>
       <c r="R145">
         <v>0</v>
@@ -5146,10 +5143,10 @@
         <v>262</v>
       </c>
       <c r="C146" s="1">
-        <v>42517.333333333336</v>
+        <v>41055.333333333336</v>
       </c>
       <c r="D146" s="1">
-        <v>42517.708333333336</v>
+        <v>41055.708333333336</v>
       </c>
       <c r="E146" t="s">
         <v>24</v>
@@ -5161,7 +5158,7 @@
         <v>0</v>
       </c>
       <c r="N146" s="1">
-        <v>42517.333333333336</v>
+        <v>41055.333333333336</v>
       </c>
     </row>
     <row r="147" spans="1:18">
@@ -5172,10 +5169,10 @@
         <v>264</v>
       </c>
       <c r="C147" s="1">
-        <v>42517.333333333336</v>
+        <v>41055.333333333336</v>
       </c>
       <c r="D147" s="1">
-        <v>42517.708333333336</v>
+        <v>41055.708333333336</v>
       </c>
       <c r="E147" t="s">
         <v>24</v>
@@ -5187,7 +5184,7 @@
         <v>0</v>
       </c>
       <c r="N147" s="1">
-        <v>42517.333333333336</v>
+        <v>41055.333333333336</v>
       </c>
       <c r="R147">
         <v>0</v>
@@ -5201,10 +5198,10 @@
         <v>266</v>
       </c>
       <c r="C148" s="1">
-        <v>42517.333333333336</v>
+        <v>41055.333333333336</v>
       </c>
       <c r="D148" s="1">
-        <v>42517.708333333336</v>
+        <v>41055.708333333336</v>
       </c>
       <c r="E148" t="s">
         <v>24</v>
@@ -5216,7 +5213,7 @@
         <v>0</v>
       </c>
       <c r="N148" s="1">
-        <v>42517.333333333336</v>
+        <v>41055.333333333336</v>
       </c>
       <c r="R148">
         <v>0</v>
@@ -5230,10 +5227,10 @@
         <v>268</v>
       </c>
       <c r="C149" s="1">
-        <v>42517.333333333336</v>
+        <v>41055.333333333336</v>
       </c>
       <c r="D149" s="1">
-        <v>42517.708333333336</v>
+        <v>41055.708333333336</v>
       </c>
       <c r="E149" t="s">
         <v>24</v>
@@ -5245,7 +5242,7 @@
         <v>0</v>
       </c>
       <c r="N149" s="1">
-        <v>42517.333333333336</v>
+        <v>41055.333333333336</v>
       </c>
       <c r="R149">
         <v>0</v>
@@ -5259,10 +5256,10 @@
         <v>270</v>
       </c>
       <c r="C150" s="1">
-        <v>42517.333333333336</v>
+        <v>41055.333333333336</v>
       </c>
       <c r="D150" s="1">
-        <v>42517.708333333336</v>
+        <v>41055.708333333336</v>
       </c>
       <c r="E150" t="s">
         <v>24</v>
@@ -5274,7 +5271,7 @@
         <v>0</v>
       </c>
       <c r="N150" s="1">
-        <v>42517.333333333336</v>
+        <v>41055.333333333336</v>
       </c>
     </row>
     <row r="151" spans="1:18">
@@ -5285,10 +5282,10 @@
         <v>273</v>
       </c>
       <c r="C151" s="1">
-        <v>42517.333333333336</v>
+        <v>41055.333333333336</v>
       </c>
       <c r="D151" s="1">
-        <v>42517.708333333336</v>
+        <v>41055.708333333336</v>
       </c>
       <c r="E151" t="s">
         <v>24</v>
@@ -5300,7 +5297,7 @@
         <v>0</v>
       </c>
       <c r="N151" s="1">
-        <v>42517.333333333336</v>
+        <v>41055.333333333336</v>
       </c>
       <c r="R151">
         <v>0</v>
@@ -5314,10 +5311,10 @@
         <v>275</v>
       </c>
       <c r="C152" s="1">
-        <v>42517.333333333336</v>
+        <v>41055.333333333336</v>
       </c>
       <c r="D152" s="1">
-        <v>42517.708333333336</v>
+        <v>41055.708333333336</v>
       </c>
       <c r="E152" t="s">
         <v>24</v>
@@ -5329,7 +5326,7 @@
         <v>0</v>
       </c>
       <c r="N152" s="1">
-        <v>42517.333333333336</v>
+        <v>41055.333333333336</v>
       </c>
       <c r="R152">
         <v>0</v>
@@ -5343,10 +5340,10 @@
         <v>276</v>
       </c>
       <c r="C153" s="1">
-        <v>42517.333333333336</v>
+        <v>41055.333333333336</v>
       </c>
       <c r="D153" s="1">
-        <v>42517.708333333336</v>
+        <v>41055.708333333336</v>
       </c>
       <c r="E153" t="s">
         <v>24</v>
@@ -5358,7 +5355,7 @@
         <v>0</v>
       </c>
       <c r="N153" s="1">
-        <v>42517.333333333336</v>
+        <v>41055.333333333336</v>
       </c>
     </row>
     <row r="154" spans="1:18">
@@ -5369,10 +5366,10 @@
         <v>278</v>
       </c>
       <c r="C154" s="1">
-        <v>42517.333333333336</v>
+        <v>41055.333333333336</v>
       </c>
       <c r="D154" s="1">
-        <v>42517.708333333336</v>
+        <v>41055.708333333336</v>
       </c>
       <c r="E154" t="s">
         <v>24</v>
@@ -5384,7 +5381,7 @@
         <v>0</v>
       </c>
       <c r="N154" s="1">
-        <v>42517.333333333336</v>
+        <v>41055.333333333336</v>
       </c>
       <c r="R154">
         <v>0</v>
@@ -5398,10 +5395,10 @@
         <v>280</v>
       </c>
       <c r="C155" s="1">
-        <v>42517.333333333336</v>
+        <v>41055.333333333336</v>
       </c>
       <c r="D155" s="1">
-        <v>42517.708333333336</v>
+        <v>41055.708333333336</v>
       </c>
       <c r="E155" t="s">
         <v>24</v>
@@ -5413,7 +5410,7 @@
         <v>0</v>
       </c>
       <c r="N155" s="1">
-        <v>42517.333333333336</v>
+        <v>41055.333333333336</v>
       </c>
       <c r="R155">
         <v>0</v>
@@ -5427,10 +5424,10 @@
         <v>282</v>
       </c>
       <c r="C156" s="1">
-        <v>42517.333333333336</v>
+        <v>41055.333333333336</v>
       </c>
       <c r="D156" s="1">
-        <v>42517.708333333336</v>
+        <v>41055.708333333336</v>
       </c>
       <c r="E156" t="s">
         <v>24</v>
@@ -5442,7 +5439,7 @@
         <v>0</v>
       </c>
       <c r="N156" s="1">
-        <v>42517.333333333336</v>
+        <v>41055.333333333336</v>
       </c>
       <c r="R156">
         <v>0</v>
@@ -5456,10 +5453,10 @@
         <v>284</v>
       </c>
       <c r="C157" s="1">
-        <v>42517.333333333336</v>
+        <v>41055.333333333336</v>
       </c>
       <c r="D157" s="1">
-        <v>42517.708333333336</v>
+        <v>41055.708333333336</v>
       </c>
       <c r="E157" t="s">
         <v>24</v>
@@ -5471,7 +5468,7 @@
         <v>0</v>
       </c>
       <c r="N157" s="1">
-        <v>42517.333333333336</v>
+        <v>41055.333333333336</v>
       </c>
       <c r="R157">
         <v>0</v>
@@ -5485,10 +5482,10 @@
         <v>285</v>
       </c>
       <c r="C158" s="1">
-        <v>42517.333333333336</v>
+        <v>41055.333333333336</v>
       </c>
       <c r="D158" s="1">
-        <v>42517.708333333336</v>
+        <v>41055.708333333336</v>
       </c>
       <c r="E158" t="s">
         <v>24</v>
@@ -5500,7 +5497,7 @@
         <v>0</v>
       </c>
       <c r="N158" s="1">
-        <v>42517.333333333336</v>
+        <v>41055.333333333336</v>
       </c>
     </row>
     <row r="159" spans="1:18">
@@ -5511,10 +5508,10 @@
         <v>287</v>
       </c>
       <c r="C159" s="1">
-        <v>42517.333333333336</v>
+        <v>41055.333333333336</v>
       </c>
       <c r="D159" s="1">
-        <v>42517.708333333336</v>
+        <v>41055.708333333336</v>
       </c>
       <c r="E159" t="s">
         <v>24</v>
@@ -5526,7 +5523,7 @@
         <v>0</v>
       </c>
       <c r="N159" s="1">
-        <v>42517.333333333336</v>
+        <v>41055.333333333336</v>
       </c>
       <c r="R159">
         <v>0</v>

</xml_diff>

<commit_message>
correction to 5.4 in workplan headings... again
</commit_message>
<xml_diff>
--- a/annex/draft_workplan/draft_workplan.xlsx
+++ b/annex/draft_workplan/draft_workplan.xlsx
@@ -474,11 +474,7 @@
     <t xml:space="preserve">Task 4. Establish a system linking unique identifiers (e.g. BS20151234) with notifications to create an integrated file register (file history) for applications within the data archive. </t>
   </si>
   <si>
-    <t xml:space="preserve">Task 5. Establish a system that: 
-a) Lists the stages in the application procedure
-b) Provides the name and contact details (within the system) for the person responsible for that stage of the procedure. 
-c) Updates the record upon completion to show the next stage in the procedure and persons responsible.
-d) Generates the permit and associated material (passes, labels, embed codes) and inform the applicant of availability by email. Accessed through the approvals section. </t>
+    <t xml:space="preserve">Task 5. Establish a system that: </t>
   </si>
   <si>
     <t>5.4.1</t>

</xml_diff>